<commit_message>
Add correcte credentials to test a happy flow of acces New test case to test the data providing from TESTNG Provider instead of XLSX file.
</commit_message>
<xml_diff>
--- a/testDataEx.xlsx
+++ b/testDataEx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amir\Desktop\Training\Selenium\Day03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amir\eclipse-workspace\TestNGSample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD39DB8-9B23-46FE-8832-E522DAFC774A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7142E9-33DE-4DA0-B90C-0C163964E5A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="2235" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4215" yWindow="3540" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,6 @@
     <t>invalid</t>
   </si>
   <si>
-    <t>mngr486459</t>
-  </si>
-  <si>
-    <t>AmEzase</t>
-  </si>
-  <si>
     <t>amir</t>
   </si>
   <si>
@@ -43,6 +37,12 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>mngr493079</t>
+  </si>
+  <si>
+    <t>zeqehEn</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -453,10 +453,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -485,10 +485,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -509,15 +509,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>1234</v>

</xml_diff>

<commit_message>
Add correct login data to test the happy flow of login. Modify the dataProvider and the user validation instructions Modify the dataProvider and the user validation instructions
</commit_message>
<xml_diff>
--- a/testDataEx.xlsx
+++ b/testDataEx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amir\eclipse-workspace\TestNGSample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7142E9-33DE-4DA0-B90C-0C163964E5A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830C2FD1-F5C4-4F3A-A1CB-BA0E17BF0B27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="3540" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15165" yWindow="690" windowWidth="8115" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -441,7 +442,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>